<commit_message>
UPDATE LAYOUT master barang multi satuan per pelanggan
</commit_message>
<xml_diff>
--- a/ImportExport/ExcelFiles/MasterBarangMultiSatuanPerPelanggan.xlsx
+++ b/ImportExport/ExcelFiles/MasterBarangMultiSatuanPerPelanggan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KERJA\AXATA\AxataPOSFilesResources\AxataPOSFilesResources\ImportExport\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8527FE36-6363-4370-8D26-E8B841C0261E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{478EB145-BBB3-4EC9-A9B7-38ED8CD0FC03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
   <si>
     <t>KATEGORI</t>
   </si>
@@ -45,9 +45,6 @@
     <t>PCS</t>
   </si>
   <si>
-    <t>NAMA</t>
-  </si>
-  <si>
     <t>JMLSTOK</t>
   </si>
   <si>
@@ -60,9 +57,6 @@
     <t>SATUAN2</t>
   </si>
   <si>
-    <t>SUPPLIER</t>
-  </si>
-  <si>
     <t>HG_UMUM1</t>
   </si>
   <si>
@@ -93,15 +87,6 @@
     <t>BARCODE</t>
   </si>
   <si>
-    <t>BARANG 1</t>
-  </si>
-  <si>
-    <t>BARANG 2</t>
-  </si>
-  <si>
-    <t>BARANG 3</t>
-  </si>
-  <si>
     <t>KATEGORI 1</t>
   </si>
   <si>
@@ -148,6 +133,21 @@
   </si>
   <si>
     <t>HG_GROSIR3</t>
+  </si>
+  <si>
+    <t>BARANG-1</t>
+  </si>
+  <si>
+    <t>BARANG-2</t>
+  </si>
+  <si>
+    <t>BARANG-3</t>
+  </si>
+  <si>
+    <t>NAMABARANG</t>
+  </si>
+  <si>
+    <t>NAMASUPPLIER</t>
   </si>
 </sst>
 </file>
@@ -606,13 +606,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Y4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2:V4"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="X9" sqref="X9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.85546875" style="10" bestFit="1" customWidth="1"/>
@@ -634,94 +634,94 @@
     <col min="20" max="20" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="15" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="10.140625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="L1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="M1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="O1" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="P1" s="5" t="s">
-        <v>18</v>
-      </c>
       <c r="Q1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="V1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="R1" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="S1" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="T1" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="U1" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="V1" s="5" t="s">
+      <c r="W1" s="5" t="s">
         <v>38</v>
-      </c>
-      <c r="W1" s="5" t="s">
-        <v>9</v>
       </c>
       <c r="X1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="Y1" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>2</v>
@@ -751,7 +751,7 @@
         <v>10</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="M2" s="1">
         <v>29000</v>
@@ -774,21 +774,21 @@
       <c r="U2" s="1"/>
       <c r="V2" s="1"/>
       <c r="W2" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="X2" s="6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="Y2" s="6" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>2</v>
@@ -815,23 +815,13 @@
         <v>42500</v>
       </c>
       <c r="K3" s="1">
-        <v>10</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="M3" s="1">
-        <v>39000</v>
-      </c>
-      <c r="N3" s="1">
-        <v>43000</v>
-      </c>
-      <c r="O3" s="1">
-        <v>42000</v>
-      </c>
-      <c r="P3" s="1">
-        <v>41000</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
       <c r="Q3" s="1">
         <v>0</v>
       </c>
@@ -841,21 +831,21 @@
       <c r="U3" s="1"/>
       <c r="V3" s="1"/>
       <c r="W3" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="X3" s="6" t="s">
         <v>2</v>
       </c>
       <c r="Y3" s="6" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>2</v>
@@ -885,7 +875,7 @@
         <v>10</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="M4" s="1">
         <v>49000</v>
@@ -908,13 +898,13 @@
       <c r="U4" s="1"/>
       <c r="V4" s="1"/>
       <c r="W4" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="X4" s="6" t="s">
         <v>2</v>
       </c>
       <c r="Y4" s="6" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update master barang multi satuan per pelanggan
</commit_message>
<xml_diff>
--- a/ImportExport/ExcelFiles/MasterBarangMultiSatuanPerPelanggan.xlsx
+++ b/ImportExport/ExcelFiles/MasterBarangMultiSatuanPerPelanggan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KERJA\AXATA\AxataPOSFilesResources\AxataPOSFilesResources\ImportExport\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{478EB145-BBB3-4EC9-A9B7-38ED8CD0FC03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E46E0AA-80CA-4FDA-94B3-780C08C9674D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
   <si>
     <t>KATEGORI</t>
   </si>
@@ -66,15 +66,9 @@
     <t>HG_GROSIR1</t>
   </si>
   <si>
-    <t>HARGABELI1</t>
-  </si>
-  <si>
     <t>SATUAN1</t>
   </si>
   <si>
-    <t>HARGABELI2</t>
-  </si>
-  <si>
     <t>HG_UMUM2</t>
   </si>
   <si>
@@ -123,9 +117,6 @@
     <t>SATUAN3</t>
   </si>
   <si>
-    <t>HARGABELI3</t>
-  </si>
-  <si>
     <t>HG_UMUM3</t>
   </si>
   <si>
@@ -135,9 +126,6 @@
     <t>HG_GROSIR3</t>
   </si>
   <si>
-    <t>BARANG-1</t>
-  </si>
-  <si>
     <t>BARANG-2</t>
   </si>
   <si>
@@ -148,6 +136,15 @@
   </si>
   <si>
     <t>NAMASUPPLIER</t>
+  </si>
+  <si>
+    <t>HARGABELI</t>
+  </si>
+  <si>
+    <t>AQUA</t>
+  </si>
+  <si>
+    <t>MINUMAN</t>
   </si>
 </sst>
 </file>
@@ -604,10 +601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Y4"/>
+  <dimension ref="A1:W4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="X9" sqref="X9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -616,47 +613,45 @@
     <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="4.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="15" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="10.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.140625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>5</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>12</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>11</v>
@@ -677,118 +672,108 @@
         <v>7</v>
       </c>
       <c r="M1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="V1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="W1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="P1" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q1" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="R1" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="S1" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="T1" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="U1" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="V1" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="W1" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="X1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y1" s="7" t="s">
-        <v>17</v>
-      </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="9">
-        <v>500</v>
+        <v>10000</v>
       </c>
       <c r="E2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="F2" s="1">
         <v>1</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="1">
-        <v>30000</v>
-      </c>
       <c r="H2" s="1">
-        <v>35000</v>
+        <v>1500</v>
       </c>
       <c r="I2" s="1">
-        <v>34000</v>
+        <v>1400</v>
       </c>
       <c r="J2" s="1">
-        <v>32500</v>
+        <v>1300</v>
       </c>
       <c r="K2" s="1">
-        <v>10</v>
+        <v>48</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M2" s="1">
-        <v>29000</v>
+        <v>55000</v>
       </c>
       <c r="N2" s="1">
-        <v>33000</v>
+        <v>54000</v>
       </c>
       <c r="O2" s="1">
-        <v>32000</v>
+        <v>53000</v>
       </c>
       <c r="P2" s="1">
-        <v>31000</v>
-      </c>
-      <c r="Q2" s="1">
         <v>0</v>
       </c>
+      <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1"/>
-      <c r="W2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="X2" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y2" s="6" t="s">
-        <v>25</v>
+      <c r="U2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="V2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="W2" s="6" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>2</v>
@@ -797,13 +782,13 @@
         <v>100</v>
       </c>
       <c r="E3" s="1">
+        <v>40000</v>
+      </c>
+      <c r="F3" s="1">
         <v>1</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="G3" s="1">
-        <v>40000</v>
       </c>
       <c r="H3" s="1">
         <v>45000</v>
@@ -821,31 +806,29 @@
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1">
+      <c r="P3" s="1">
         <v>0</v>
       </c>
+      <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
-      <c r="U3" s="1"/>
-      <c r="V3" s="1"/>
-      <c r="W3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="X3" s="6" t="s">
+      <c r="U3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="V3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="Y3" s="6" t="s">
-        <v>24</v>
+      <c r="W3" s="6" t="s">
+        <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>2</v>
@@ -854,13 +837,13 @@
         <v>300</v>
       </c>
       <c r="E4" s="1">
+        <v>50000</v>
+      </c>
+      <c r="F4" s="1">
         <v>1</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="G4" s="1">
-        <v>50000</v>
       </c>
       <c r="H4" s="1">
         <v>55000</v>
@@ -875,36 +858,32 @@
         <v>10</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M4" s="1">
-        <v>49000</v>
+        <v>53000</v>
       </c>
       <c r="N4" s="1">
-        <v>53000</v>
+        <v>52000</v>
       </c>
       <c r="O4" s="1">
-        <v>52000</v>
+        <v>51000</v>
       </c>
       <c r="P4" s="1">
-        <v>51000</v>
-      </c>
-      <c r="Q4" s="1">
         <v>0</v>
       </c>
+      <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
-      <c r="U4" s="1"/>
-      <c r="V4" s="1"/>
-      <c r="W4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="X4" s="6" t="s">
+      <c r="U4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="V4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="Y4" s="6" t="s">
-        <v>23</v>
+      <c r="W4" s="6" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>